<commit_message>
Fixed Bugs created by evil machine overlords
</commit_message>
<xml_diff>
--- a/0_0_Data/3_Naive_Forecaster_Data/1_QoQ_Forecast_Tables/naive_qoq_forecasts_AVERAGE_10_9.xlsx
+++ b/0_0_Data/3_Naive_Forecaster_Data/1_QoQ_Forecast_Tables/naive_qoq_forecasts_AVERAGE_10_9.xlsx
@@ -826,7 +826,7 @@
     </row>
     <row r="2" spans="1:150">
       <c r="A2" s="1">
-        <v>32509</v>
+        <v>32417</v>
       </c>
       <c r="B2">
         <v>0.6941229168137555</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="3" spans="1:150">
       <c r="A3" s="1">
-        <v>32599</v>
+        <v>32509</v>
       </c>
       <c r="B3">
         <v>0.6941229168137555</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="4" spans="1:150">
       <c r="A4" s="1">
-        <v>32690</v>
+        <v>32599</v>
       </c>
       <c r="B4">
         <v>0.6941229168137555</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="5" spans="1:150">
       <c r="A5" s="1">
-        <v>32782</v>
+        <v>32690</v>
       </c>
       <c r="B5">
         <v>0.6941229168137555</v>
@@ -876,7 +876,7 @@
     </row>
     <row r="6" spans="1:150">
       <c r="A6" s="1">
-        <v>32874</v>
+        <v>32782</v>
       </c>
       <c r="B6">
         <v>0.6941229168137555</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="7" spans="1:150">
       <c r="A7" s="1">
-        <v>32964</v>
+        <v>32874</v>
       </c>
       <c r="B7">
         <v>0.6941229168137555</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="8" spans="1:150">
       <c r="A8" s="1">
-        <v>33055</v>
+        <v>32964</v>
       </c>
       <c r="B8">
         <v>0.6941229168137555</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="9" spans="1:150">
       <c r="A9" s="1">
-        <v>33147</v>
+        <v>33055</v>
       </c>
       <c r="B9">
         <v>0.6941229168137555</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="10" spans="1:150">
       <c r="A10" s="1">
-        <v>33239</v>
+        <v>33147</v>
       </c>
       <c r="B10">
         <v>0.6941229168137555</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="11" spans="1:150">
       <c r="A11" s="1">
-        <v>33329</v>
+        <v>33239</v>
       </c>
       <c r="B11">
         <v>0.6941229168137555</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="12" spans="1:150">
       <c r="A12" s="1">
-        <v>33420</v>
+        <v>33329</v>
       </c>
       <c r="C12">
         <v>0.6977962488903545</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="13" spans="1:150">
       <c r="A13" s="1">
-        <v>33512</v>
+        <v>33420</v>
       </c>
       <c r="D13">
         <v>0.7265532797071169</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="14" spans="1:150">
       <c r="A14" s="1">
-        <v>33604</v>
+        <v>33512</v>
       </c>
       <c r="E14">
         <v>0.6689726032975558</v>
@@ -1146,7 +1146,7 @@
     </row>
     <row r="15" spans="1:150">
       <c r="A15" s="1">
-        <v>33695</v>
+        <v>33604</v>
       </c>
       <c r="F15">
         <v>1.010411931874227</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="16" spans="1:150">
       <c r="A16" s="1">
-        <v>33786</v>
+        <v>33695</v>
       </c>
       <c r="G16">
         <v>0.9028466069939436</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="17" spans="1:32">
       <c r="A17" s="1">
-        <v>33878</v>
+        <v>33786</v>
       </c>
       <c r="H17">
         <v>1.039122700114349</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="18" spans="1:32">
       <c r="A18" s="1">
-        <v>33970</v>
+        <v>33878</v>
       </c>
       <c r="I18">
         <v>0.9296537578982891</v>
@@ -1286,7 +1286,7 @@
     </row>
     <row r="19" spans="1:32">
       <c r="A19" s="1">
-        <v>34060</v>
+        <v>33970</v>
       </c>
       <c r="J19">
         <v>1.230223668275899</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="20" spans="1:32">
       <c r="A20" s="1">
-        <v>34151</v>
+        <v>34060</v>
       </c>
       <c r="K20">
         <v>1.225558682898375</v>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="21" spans="1:32">
       <c r="A21" s="1">
-        <v>34243</v>
+        <v>34151</v>
       </c>
       <c r="L21">
         <v>1.391546652594672</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="22" spans="1:32">
       <c r="A22" s="1">
-        <v>34335</v>
+        <v>34243</v>
       </c>
       <c r="M22">
         <v>1.382895392343677</v>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="23" spans="1:32">
       <c r="A23" s="1">
-        <v>34425</v>
+        <v>34335</v>
       </c>
       <c r="N23">
         <v>1.220384266219</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="24" spans="1:32">
       <c r="A24" s="1">
-        <v>34516</v>
+        <v>34425</v>
       </c>
       <c r="O24">
         <v>1.266097133135795</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="25" spans="1:32">
       <c r="A25" s="1">
-        <v>34608</v>
+        <v>34516</v>
       </c>
       <c r="P25">
         <v>1.310921819859853</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="26" spans="1:32">
       <c r="A26" s="1">
-        <v>34700</v>
+        <v>34608</v>
       </c>
       <c r="Q26">
         <v>1.189380007335642</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="27" spans="1:32">
       <c r="A27" s="1">
-        <v>34790</v>
+        <v>34700</v>
       </c>
       <c r="R27">
         <v>0.9669164196629385</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="28" spans="1:32">
       <c r="A28" s="1">
-        <v>34881</v>
+        <v>34790</v>
       </c>
       <c r="S28">
         <v>0.9046564641343317</v>
@@ -1636,7 +1636,7 @@
     </row>
     <row r="29" spans="1:32">
       <c r="A29" s="1">
-        <v>34973</v>
+        <v>34881</v>
       </c>
       <c r="T29">
         <v>0.5144912346401558</v>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="30" spans="1:32">
       <c r="A30" s="1">
-        <v>35065</v>
+        <v>34973</v>
       </c>
       <c r="U30">
         <v>0.4002556464150967</v>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="31" spans="1:32">
       <c r="A31" s="1">
-        <v>35156</v>
+        <v>35065</v>
       </c>
       <c r="V31">
         <v>0.196837000609057</v>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="32" spans="1:32">
       <c r="A32" s="1">
-        <v>35247</v>
+        <v>35156</v>
       </c>
       <c r="W32">
         <v>0.06611687940479796</v>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="33" spans="1:48">
       <c r="A33" s="1">
-        <v>35339</v>
+        <v>35247</v>
       </c>
       <c r="X33">
         <v>0.2438250556392446</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="34" spans="1:48">
       <c r="A34" s="1">
-        <v>35431</v>
+        <v>35339</v>
       </c>
       <c r="Y34">
         <v>0.28010555977989</v>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="35" spans="1:48">
       <c r="A35" s="1">
-        <v>35521</v>
+        <v>35431</v>
       </c>
       <c r="Z35">
         <v>0.207454499574576</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="36" spans="1:48">
       <c r="A36" s="1">
-        <v>35612</v>
+        <v>35521</v>
       </c>
       <c r="AA36">
         <v>0.2734065588080321</v>
@@ -1916,7 +1916,7 @@
     </row>
     <row r="37" spans="1:48">
       <c r="A37" s="1">
-        <v>35704</v>
+        <v>35612</v>
       </c>
       <c r="AB37">
         <v>0.3098800914713071</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="38" spans="1:48">
       <c r="A38" s="1">
-        <v>35796</v>
+        <v>35704</v>
       </c>
       <c r="AC38">
         <v>0.4302782422791499</v>
@@ -1986,7 +1986,7 @@
     </row>
     <row r="39" spans="1:48">
       <c r="A39" s="1">
-        <v>35886</v>
+        <v>35796</v>
       </c>
       <c r="AD39">
         <v>0.6078992789691108</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="40" spans="1:48">
       <c r="A40" s="1">
-        <v>35977</v>
+        <v>35886</v>
       </c>
       <c r="AE40">
         <v>0.5211670451689333</v>
@@ -2056,7 +2056,7 @@
     </row>
     <row r="41" spans="1:48">
       <c r="A41" s="1">
-        <v>36069</v>
+        <v>35977</v>
       </c>
       <c r="AF41">
         <v>0.4316829867807276</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="42" spans="1:48">
       <c r="A42" s="1">
-        <v>36161</v>
+        <v>36069</v>
       </c>
       <c r="AG42">
         <v>0.5660059002693849</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="43" spans="1:48">
       <c r="A43" s="1">
-        <v>36251</v>
+        <v>36161</v>
       </c>
       <c r="AH43">
         <v>0.5293349251255315</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="44" spans="1:48">
       <c r="A44" s="1">
-        <v>36342</v>
+        <v>36251</v>
       </c>
       <c r="AI44">
         <v>0.4513582675054688</v>
@@ -2196,7 +2196,7 @@
     </row>
     <row r="45" spans="1:48">
       <c r="A45" s="1">
-        <v>36434</v>
+        <v>36342</v>
       </c>
       <c r="AJ45">
         <v>0.4385008674071109</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="46" spans="1:48">
       <c r="A46" s="1">
-        <v>36526</v>
+        <v>36434</v>
       </c>
       <c r="AK46">
         <v>0.413380026209433</v>
@@ -2266,7 +2266,7 @@
     </row>
     <row r="47" spans="1:48">
       <c r="A47" s="1">
-        <v>36617</v>
+        <v>36526</v>
       </c>
       <c r="AL47">
         <v>0.4658116210677422</v>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="48" spans="1:48">
       <c r="A48" s="1">
-        <v>36708</v>
+        <v>36617</v>
       </c>
       <c r="AM48">
         <v>0.4181062710828364</v>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="49" spans="1:64">
       <c r="A49" s="1">
-        <v>36800</v>
+        <v>36708</v>
       </c>
       <c r="AN49">
         <v>0.5384412360130529</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="50" spans="1:64">
       <c r="A50" s="1">
-        <v>36892</v>
+        <v>36800</v>
       </c>
       <c r="AO50">
         <v>0.5927126047459808</v>
@@ -2406,7 +2406,7 @@
     </row>
     <row r="51" spans="1:64">
       <c r="A51" s="1">
-        <v>36982</v>
+        <v>36892</v>
       </c>
       <c r="AP51">
         <v>0.6706807844985097</v>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="52" spans="1:64">
       <c r="A52" s="1">
-        <v>37073</v>
+        <v>36982</v>
       </c>
       <c r="AQ52">
         <v>0.4946468788584245</v>
@@ -2476,7 +2476,7 @@
     </row>
     <row r="53" spans="1:64">
       <c r="A53" s="1">
-        <v>37165</v>
+        <v>37073</v>
       </c>
       <c r="AR53">
         <v>0.3934033285524757</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="54" spans="1:64">
       <c r="A54" s="1">
-        <v>37257</v>
+        <v>37165</v>
       </c>
       <c r="AS54">
         <v>0.3112293886097183</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="55" spans="1:64">
       <c r="A55" s="1">
-        <v>37347</v>
+        <v>37257</v>
       </c>
       <c r="AT55">
         <v>0.455531728878449</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="56" spans="1:64">
       <c r="A56" s="1">
-        <v>37438</v>
+        <v>37347</v>
       </c>
       <c r="AU56">
         <v>0.4247769310011789</v>
@@ -2616,7 +2616,7 @@
     </row>
     <row r="57" spans="1:64">
       <c r="A57" s="1">
-        <v>37530</v>
+        <v>37438</v>
       </c>
       <c r="AV57">
         <v>0.4582009035931788</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="58" spans="1:64">
       <c r="A58" s="1">
-        <v>37622</v>
+        <v>37530</v>
       </c>
       <c r="AW58">
         <v>0.52853566461182</v>
@@ -2686,7 +2686,7 @@
     </row>
     <row r="59" spans="1:64">
       <c r="A59" s="1">
-        <v>37712</v>
+        <v>37622</v>
       </c>
       <c r="AX59">
         <v>0.4797652918828937</v>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="60" spans="1:64">
       <c r="A60" s="1">
-        <v>37803</v>
+        <v>37712</v>
       </c>
       <c r="AY60">
         <v>0.5372636768001781</v>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="61" spans="1:64">
       <c r="A61" s="1">
-        <v>37895</v>
+        <v>37803</v>
       </c>
       <c r="AZ61">
         <v>0.5446302776114635</v>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="62" spans="1:64">
       <c r="A62" s="1">
-        <v>37987</v>
+        <v>37895</v>
       </c>
       <c r="BA62">
         <v>0.584225439885914</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="63" spans="1:64">
       <c r="A63" s="1">
-        <v>38078</v>
+        <v>37987</v>
       </c>
       <c r="BB63">
         <v>0.4577438289507324</v>
@@ -2861,7 +2861,7 @@
     </row>
     <row r="64" spans="1:64">
       <c r="A64" s="1">
-        <v>38169</v>
+        <v>38078</v>
       </c>
       <c r="BC64">
         <v>0.4573018825487105</v>
@@ -2896,7 +2896,7 @@
     </row>
     <row r="65" spans="1:80">
       <c r="A65" s="1">
-        <v>38261</v>
+        <v>38169</v>
       </c>
       <c r="BD65">
         <v>0.3487543934966478</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="66" spans="1:80">
       <c r="A66" s="1">
-        <v>38353</v>
+        <v>38261</v>
       </c>
       <c r="BE66">
         <v>0.255281228968523</v>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="67" spans="1:80">
       <c r="A67" s="1">
-        <v>38443</v>
+        <v>38353</v>
       </c>
       <c r="BF67">
         <v>0.196079099379528</v>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="68" spans="1:80">
       <c r="A68" s="1">
-        <v>38534</v>
+        <v>38443</v>
       </c>
       <c r="BG68">
         <v>0.09136230502795779</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="69" spans="1:80">
       <c r="A69" s="1">
-        <v>38626</v>
+        <v>38534</v>
       </c>
       <c r="BH69">
         <v>0.06399930331093673</v>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="70" spans="1:80">
       <c r="A70" s="1">
-        <v>38718</v>
+        <v>38626</v>
       </c>
       <c r="BI70">
         <v>0.07334711583925703</v>
@@ -3106,7 +3106,7 @@
     </row>
     <row r="71" spans="1:80">
       <c r="A71" s="1">
-        <v>38808</v>
+        <v>38718</v>
       </c>
       <c r="BJ71">
         <v>-6.049006130520729E-05</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="72" spans="1:80">
       <c r="A72" s="1">
-        <v>38899</v>
+        <v>38808</v>
       </c>
       <c r="BK72">
         <v>0.02123607104907491</v>
@@ -3176,7 +3176,7 @@
     </row>
     <row r="73" spans="1:80">
       <c r="A73" s="1">
-        <v>38991</v>
+        <v>38899</v>
       </c>
       <c r="BL73">
         <v>0.08464689759247299</v>
@@ -3211,7 +3211,7 @@
     </row>
     <row r="74" spans="1:80">
       <c r="A74" s="1">
-        <v>39083</v>
+        <v>38991</v>
       </c>
       <c r="BM74">
         <v>0.139984886153875</v>
@@ -3246,7 +3246,7 @@
     </row>
     <row r="75" spans="1:80">
       <c r="A75" s="1">
-        <v>39173</v>
+        <v>39083</v>
       </c>
       <c r="BN75">
         <v>0.1403118607824707</v>
@@ -3281,7 +3281,7 @@
     </row>
     <row r="76" spans="1:80">
       <c r="A76" s="1">
-        <v>39264</v>
+        <v>39173</v>
       </c>
       <c r="BO76">
         <v>0.08973464093123734</v>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="77" spans="1:80">
       <c r="A77" s="1">
-        <v>39356</v>
+        <v>39264</v>
       </c>
       <c r="BP77">
         <v>0.1664705992650774</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="78" spans="1:80">
       <c r="A78" s="1">
-        <v>39448</v>
+        <v>39356</v>
       </c>
       <c r="BQ78">
         <v>0.139526942479626</v>
@@ -3386,7 +3386,7 @@
     </row>
     <row r="79" spans="1:80">
       <c r="A79" s="1">
-        <v>39539</v>
+        <v>39448</v>
       </c>
       <c r="BR79">
         <v>0.2663255547813869</v>
@@ -3421,7 +3421,7 @@
     </row>
     <row r="80" spans="1:80">
       <c r="A80" s="1">
-        <v>39630</v>
+        <v>39539</v>
       </c>
       <c r="BS80">
         <v>0.2927776881228313</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="81" spans="1:96">
       <c r="A81" s="1">
-        <v>39722</v>
+        <v>39630</v>
       </c>
       <c r="BT81">
         <v>0.3072286933641231</v>
@@ -3491,7 +3491,7 @@
     </row>
     <row r="82" spans="1:96">
       <c r="A82" s="1">
-        <v>39814</v>
+        <v>39722</v>
       </c>
       <c r="BU82">
         <v>0.3432290764637597</v>
@@ -3526,7 +3526,7 @@
     </row>
     <row r="83" spans="1:96">
       <c r="A83" s="1">
-        <v>39904</v>
+        <v>39814</v>
       </c>
       <c r="BV83">
         <v>0.3980203508502676</v>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="84" spans="1:96">
       <c r="A84" s="1">
-        <v>39995</v>
+        <v>39904</v>
       </c>
       <c r="BW84">
         <v>0.5254668165067387</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="85" spans="1:96">
       <c r="A85" s="1">
-        <v>40087</v>
+        <v>39995</v>
       </c>
       <c r="BX85">
         <v>0.611889475066235</v>
@@ -3631,7 +3631,7 @@
     </row>
     <row r="86" spans="1:96">
       <c r="A86" s="1">
-        <v>40179</v>
+        <v>40087</v>
       </c>
       <c r="BY86">
         <v>0.6294852851196401</v>
@@ -3666,7 +3666,7 @@
     </row>
     <row r="87" spans="1:96">
       <c r="A87" s="1">
-        <v>40269</v>
+        <v>40179</v>
       </c>
       <c r="BZ87">
         <v>0.6624312234319696</v>
@@ -3701,7 +3701,7 @@
     </row>
     <row r="88" spans="1:96">
       <c r="A88" s="1">
-        <v>40360</v>
+        <v>40269</v>
       </c>
       <c r="CA88">
         <v>0.6479710228601918</v>
@@ -3736,7 +3736,7 @@
     </row>
     <row r="89" spans="1:96">
       <c r="A89" s="1">
-        <v>40452</v>
+        <v>40360</v>
       </c>
       <c r="CB89">
         <v>0.7441680314761443</v>
@@ -3771,7 +3771,7 @@
     </row>
     <row r="90" spans="1:96">
       <c r="A90" s="1">
-        <v>40544</v>
+        <v>40452</v>
       </c>
       <c r="CC90">
         <v>0.6547901257702069</v>
@@ -3806,7 +3806,7 @@
     </row>
     <row r="91" spans="1:96">
       <c r="A91" s="1">
-        <v>40634</v>
+        <v>40544</v>
       </c>
       <c r="CD91">
         <v>0.5383282916003549</v>
@@ -3841,7 +3841,7 @@
     </row>
     <row r="92" spans="1:96">
       <c r="A92" s="1">
-        <v>40725</v>
+        <v>40634</v>
       </c>
       <c r="CE92">
         <v>0.1818297597035944</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="93" spans="1:96">
       <c r="A93" s="1">
-        <v>40817</v>
+        <v>40725</v>
       </c>
       <c r="CF93">
         <v>-0.2799684307986602</v>
@@ -3911,7 +3911,7 @@
     </row>
     <row r="94" spans="1:96">
       <c r="A94" s="1">
-        <v>40909</v>
+        <v>40817</v>
       </c>
       <c r="CG94">
         <v>-0.3373491821102736</v>
@@ -3946,7 +3946,7 @@
     </row>
     <row r="95" spans="1:96">
       <c r="A95" s="1">
-        <v>41000</v>
+        <v>40909</v>
       </c>
       <c r="CH95">
         <v>-0.2844562691596675</v>
@@ -3981,7 +3981,7 @@
     </row>
     <row r="96" spans="1:96">
       <c r="A96" s="1">
-        <v>41091</v>
+        <v>41000</v>
       </c>
       <c r="CI96">
         <v>-0.3139862207927315</v>
@@ -4016,7 +4016,7 @@
     </row>
     <row r="97" spans="1:112">
       <c r="A97" s="1">
-        <v>41183</v>
+        <v>41091</v>
       </c>
       <c r="CJ97">
         <v>-0.3608021799647745</v>
@@ -4051,7 +4051,7 @@
     </row>
     <row r="98" spans="1:112">
       <c r="A98" s="1">
-        <v>41275</v>
+        <v>41183</v>
       </c>
       <c r="CK98">
         <v>-0.12628722994408</v>
@@ -4086,7 +4086,7 @@
     </row>
     <row r="99" spans="1:112">
       <c r="A99" s="1">
-        <v>41365</v>
+        <v>41275</v>
       </c>
       <c r="CL99">
         <v>-0.1703233649732007</v>
@@ -4121,7 +4121,7 @@
     </row>
     <row r="100" spans="1:112">
       <c r="A100" s="1">
-        <v>41456</v>
+        <v>41365</v>
       </c>
       <c r="CM100">
         <v>-0.06497206438053668</v>
@@ -4156,7 +4156,7 @@
     </row>
     <row r="101" spans="1:112">
       <c r="A101" s="1">
-        <v>41548</v>
+        <v>41456</v>
       </c>
       <c r="CN101">
         <v>0.1305915191252485</v>
@@ -4191,7 +4191,7 @@
     </row>
     <row r="102" spans="1:112">
       <c r="A102" s="1">
-        <v>41640</v>
+        <v>41548</v>
       </c>
       <c r="CO102">
         <v>0.3040734292842707</v>
@@ -4226,7 +4226,7 @@
     </row>
     <row r="103" spans="1:112">
       <c r="A103" s="1">
-        <v>41730</v>
+        <v>41640</v>
       </c>
       <c r="CP103">
         <v>0.7707958028869695</v>
@@ -4261,7 +4261,7 @@
     </row>
     <row r="104" spans="1:112">
       <c r="A104" s="1">
-        <v>41821</v>
+        <v>41730</v>
       </c>
       <c r="CQ104">
         <v>0.728485290145509</v>
@@ -4296,7 +4296,7 @@
     </row>
     <row r="105" spans="1:112">
       <c r="A105" s="1">
-        <v>41913</v>
+        <v>41821</v>
       </c>
       <c r="CR105">
         <v>0.6982082002245201</v>
@@ -4331,7 +4331,7 @@
     </row>
     <row r="106" spans="1:112">
       <c r="A106" s="1">
-        <v>42005</v>
+        <v>41913</v>
       </c>
       <c r="CS106">
         <v>0.685593016150544</v>
@@ -4366,7 +4366,7 @@
     </row>
     <row r="107" spans="1:112">
       <c r="A107" s="1">
-        <v>42095</v>
+        <v>42005</v>
       </c>
       <c r="CT107">
         <v>0.642517155860985</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="108" spans="1:112">
       <c r="A108" s="1">
-        <v>42186</v>
+        <v>42095</v>
       </c>
       <c r="CU108">
         <v>0.3630944065379357</v>
@@ -4436,7 +4436,7 @@
     </row>
     <row r="109" spans="1:112">
       <c r="A109" s="1">
-        <v>42278</v>
+        <v>42186</v>
       </c>
       <c r="CV109">
         <v>0.2884579956870195</v>
@@ -4471,7 +4471,7 @@
     </row>
     <row r="110" spans="1:112">
       <c r="A110" s="1">
-        <v>42370</v>
+        <v>42278</v>
       </c>
       <c r="CW110">
         <v>0.3193273013225455</v>
@@ -4506,7 +4506,7 @@
     </row>
     <row r="111" spans="1:112">
       <c r="A111" s="1">
-        <v>42461</v>
+        <v>42370</v>
       </c>
       <c r="CX111">
         <v>0.1981397788874456</v>
@@ -4541,7 +4541,7 @@
     </row>
     <row r="112" spans="1:112">
       <c r="A112" s="1">
-        <v>42552</v>
+        <v>42461</v>
       </c>
       <c r="CY112">
         <v>0.2274130099267809</v>
@@ -4576,7 +4576,7 @@
     </row>
     <row r="113" spans="1:128">
       <c r="A113" s="1">
-        <v>42644</v>
+        <v>42552</v>
       </c>
       <c r="CZ113">
         <v>0.2664625129919059</v>
@@ -4611,7 +4611,7 @@
     </row>
     <row r="114" spans="1:128">
       <c r="A114" s="1">
-        <v>42736</v>
+        <v>42644</v>
       </c>
       <c r="DA114">
         <v>0.1749360396833936</v>
@@ -4646,7 +4646,7 @@
     </row>
     <row r="115" spans="1:128">
       <c r="A115" s="1">
-        <v>42826</v>
+        <v>42736</v>
       </c>
       <c r="DB115">
         <v>0.1678009349620006</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="116" spans="1:128">
       <c r="A116" s="1">
-        <v>42917</v>
+        <v>42826</v>
       </c>
       <c r="DC116">
         <v>0.2262235086062239</v>
@@ -4716,7 +4716,7 @@
     </row>
     <row r="117" spans="1:128">
       <c r="A117" s="1">
-        <v>43009</v>
+        <v>42917</v>
       </c>
       <c r="DD117">
         <v>0.2448105132036734</v>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="118" spans="1:128">
       <c r="A118" s="1">
-        <v>43101</v>
+        <v>43009</v>
       </c>
       <c r="DE118">
         <v>0.3577719600750547</v>
@@ -4786,7 +4786,7 @@
     </row>
     <row r="119" spans="1:128">
       <c r="A119" s="1">
-        <v>43191</v>
+        <v>43101</v>
       </c>
       <c r="DF119">
         <v>0.4163265652198342</v>
@@ -4821,7 +4821,7 @@
     </row>
     <row r="120" spans="1:128">
       <c r="A120" s="1">
-        <v>43282</v>
+        <v>43191</v>
       </c>
       <c r="DG120">
         <v>0.3496473259638563</v>
@@ -4856,7 +4856,7 @@
     </row>
     <row r="121" spans="1:128">
       <c r="A121" s="1">
-        <v>43374</v>
+        <v>43282</v>
       </c>
       <c r="DH121">
         <v>0.3788614630760844</v>
@@ -4891,7 +4891,7 @@
     </row>
     <row r="122" spans="1:128">
       <c r="A122" s="1">
-        <v>43466</v>
+        <v>43374</v>
       </c>
       <c r="DI122">
         <v>0.3975045438070423</v>
@@ -4926,7 +4926,7 @@
     </row>
     <row r="123" spans="1:128">
       <c r="A123" s="1">
-        <v>43556</v>
+        <v>43466</v>
       </c>
       <c r="DJ123">
         <v>0.3569589506680418</v>
@@ -4961,7 +4961,7 @@
     </row>
     <row r="124" spans="1:128">
       <c r="A124" s="1">
-        <v>43647</v>
+        <v>43556</v>
       </c>
       <c r="DK124">
         <v>0.41093607707931</v>
@@ -4996,7 +4996,7 @@
     </row>
     <row r="125" spans="1:128">
       <c r="A125" s="1">
-        <v>43739</v>
+        <v>43647</v>
       </c>
       <c r="DL125">
         <v>0.4450648425140112</v>
@@ -5031,7 +5031,7 @@
     </row>
     <row r="126" spans="1:128">
       <c r="A126" s="1">
-        <v>43831</v>
+        <v>43739</v>
       </c>
       <c r="DM126">
         <v>0.4478334266741417</v>
@@ -5066,7 +5066,7 @@
     </row>
     <row r="127" spans="1:128">
       <c r="A127" s="1">
-        <v>43922</v>
+        <v>43831</v>
       </c>
       <c r="DN127">
         <v>0.5387779590805554</v>
@@ -5101,7 +5101,7 @@
     </row>
     <row r="128" spans="1:128">
       <c r="A128" s="1">
-        <v>44013</v>
+        <v>43922</v>
       </c>
       <c r="DO128">
         <v>0.5469815053509908</v>
@@ -5136,7 +5136,7 @@
     </row>
     <row r="129" spans="1:144">
       <c r="A129" s="1">
-        <v>44105</v>
+        <v>44013</v>
       </c>
       <c r="DP129">
         <v>0.5443919446995226</v>
@@ -5171,7 +5171,7 @@
     </row>
     <row r="130" spans="1:144">
       <c r="A130" s="1">
-        <v>44197</v>
+        <v>44105</v>
       </c>
       <c r="DQ130">
         <v>0.5509252772825745</v>
@@ -5206,7 +5206,7 @@
     </row>
     <row r="131" spans="1:144">
       <c r="A131" s="1">
-        <v>44287</v>
+        <v>44197</v>
       </c>
       <c r="DR131">
         <v>0.4397085823035038</v>
@@ -5241,7 +5241,7 @@
     </row>
     <row r="132" spans="1:144">
       <c r="A132" s="1">
-        <v>44378</v>
+        <v>44287</v>
       </c>
       <c r="DS132">
         <v>0.3979624383165997</v>
@@ -5276,7 +5276,7 @@
     </row>
     <row r="133" spans="1:144">
       <c r="A133" s="1">
-        <v>44470</v>
+        <v>44378</v>
       </c>
       <c r="DT133">
         <v>0.4232775010493146</v>
@@ -5311,7 +5311,7 @@
     </row>
     <row r="134" spans="1:144">
       <c r="A134" s="1">
-        <v>44562</v>
+        <v>44470</v>
       </c>
       <c r="DU134">
         <v>0.4273161660922285</v>
@@ -5346,7 +5346,7 @@
     </row>
     <row r="135" spans="1:144">
       <c r="A135" s="1">
-        <v>44652</v>
+        <v>44562</v>
       </c>
       <c r="DV135">
         <v>0.3084390294012061</v>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="136" spans="1:144">
       <c r="A136" s="1">
-        <v>44743</v>
+        <v>44652</v>
       </c>
       <c r="DW136">
         <v>0.2675153907458341</v>
@@ -5416,7 +5416,7 @@
     </row>
     <row r="137" spans="1:144">
       <c r="A137" s="1">
-        <v>44835</v>
+        <v>44743</v>
       </c>
       <c r="DX137">
         <v>-0.04740977767513747</v>
@@ -5451,7 +5451,7 @@
     </row>
     <row r="138" spans="1:144">
       <c r="A138" s="1">
-        <v>44927</v>
+        <v>44835</v>
       </c>
       <c r="DY138">
         <v>-1.103784737857667</v>
@@ -5486,7 +5486,7 @@
     </row>
     <row r="139" spans="1:144">
       <c r="A139" s="1">
-        <v>45017</v>
+        <v>44927</v>
       </c>
       <c r="DZ139">
         <v>-0.2331383618867365</v>
@@ -5521,7 +5521,7 @@
     </row>
     <row r="140" spans="1:144">
       <c r="A140" s="1">
-        <v>45108</v>
+        <v>45017</v>
       </c>
       <c r="EA140">
         <v>-0.24378957821662</v>
@@ -5556,7 +5556,7 @@
     </row>
     <row r="141" spans="1:144">
       <c r="A141" s="1">
-        <v>45200</v>
+        <v>45108</v>
       </c>
       <c r="EB141">
         <v>-0.3524041104327608</v>
@@ -5591,7 +5591,7 @@
     </row>
     <row r="142" spans="1:144">
       <c r="A142" s="1">
-        <v>45292</v>
+        <v>45200</v>
       </c>
       <c r="EC142">
         <v>-0.1443023894650218</v>
@@ -5626,7 +5626,7 @@
     </row>
     <row r="143" spans="1:144">
       <c r="A143" s="1">
-        <v>45383</v>
+        <v>45292</v>
       </c>
       <c r="ED143">
         <v>-0.02780421909122137</v>
@@ -5661,7 +5661,7 @@
     </row>
     <row r="144" spans="1:144">
       <c r="A144" s="1">
-        <v>45474</v>
+        <v>45383</v>
       </c>
       <c r="EE144">
         <v>0.01768919490591373</v>
@@ -5696,7 +5696,7 @@
     </row>
     <row r="145" spans="1:150">
       <c r="A145" s="1">
-        <v>45566</v>
+        <v>45474</v>
       </c>
       <c r="EF145">
         <v>0.0001350735459492769</v>
@@ -5731,7 +5731,7 @@
     </row>
     <row r="146" spans="1:150">
       <c r="A146" s="1">
-        <v>45658</v>
+        <v>45566</v>
       </c>
       <c r="EG146">
         <v>0.08824239249695551</v>
@@ -5766,7 +5766,7 @@
     </row>
     <row r="147" spans="1:150">
       <c r="A147" s="1">
-        <v>45748</v>
+        <v>45658</v>
       </c>
       <c r="EH147">
         <v>0.2668170259847391</v>
@@ -5801,7 +5801,7 @@
     </row>
     <row r="148" spans="1:150">
       <c r="A148" s="1">
-        <v>45839</v>
+        <v>45748</v>
       </c>
       <c r="EI148">
         <v>1.178844253737389</v>
@@ -5836,7 +5836,7 @@
     </row>
     <row r="149" spans="1:150">
       <c r="A149" s="1">
-        <v>45931</v>
+        <v>45839</v>
       </c>
       <c r="EJ149">
         <v>0.2348700177716323</v>
@@ -5871,7 +5871,7 @@
     </row>
     <row r="150" spans="1:150">
       <c r="A150" s="1">
-        <v>46023</v>
+        <v>45931</v>
       </c>
       <c r="EK150">
         <v>0.2388379152847414</v>
@@ -5906,7 +5906,7 @@
     </row>
     <row r="151" spans="1:150">
       <c r="A151" s="1">
-        <v>46113</v>
+        <v>46023</v>
       </c>
       <c r="EL151">
         <v>0.3744780054549828</v>
@@ -5938,7 +5938,7 @@
     </row>
     <row r="152" spans="1:150">
       <c r="A152" s="1">
-        <v>46204</v>
+        <v>46113</v>
       </c>
       <c r="EM152">
         <v>0.1336718235993181</v>
@@ -5967,7 +5967,7 @@
     </row>
     <row r="153" spans="1:150">
       <c r="A153" s="1">
-        <v>46296</v>
+        <v>46204</v>
       </c>
       <c r="EN153">
         <v>0.08834060834722172</v>
@@ -5993,7 +5993,7 @@
     </row>
     <row r="154" spans="1:150">
       <c r="A154" s="1">
-        <v>46388</v>
+        <v>46296</v>
       </c>
       <c r="EO154">
         <v>0.02147918641116785</v>
@@ -6016,7 +6016,7 @@
     </row>
     <row r="155" spans="1:150">
       <c r="A155" s="1">
-        <v>46478</v>
+        <v>46388</v>
       </c>
       <c r="EP155">
         <v>-0.00810701594554874</v>
@@ -6036,7 +6036,7 @@
     </row>
     <row r="156" spans="1:150">
       <c r="A156" s="1">
-        <v>46569</v>
+        <v>46478</v>
       </c>
       <c r="EQ156">
         <v>-0.02625767267518964</v>
@@ -6053,7 +6053,7 @@
     </row>
     <row r="157" spans="1:150">
       <c r="A157" s="1">
-        <v>46661</v>
+        <v>46569</v>
       </c>
       <c r="ER157">
         <v>-0.04428949692388896</v>
@@ -6067,7 +6067,7 @@
     </row>
     <row r="158" spans="1:150">
       <c r="A158" s="1">
-        <v>46753</v>
+        <v>46661</v>
       </c>
       <c r="ES158">
         <v>-0.09587373626955231</v>
@@ -6078,7 +6078,7 @@
     </row>
     <row r="159" spans="1:150">
       <c r="A159" s="1">
-        <v>46844</v>
+        <v>46753</v>
       </c>
       <c r="ET159">
         <v>-0.04181509226822702</v>

</xml_diff>